<commit_message>
mise a jour JNLTRAV
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_MateenKhalil.xlsx
+++ b/Doc/Journal-de-Travail_MateenKhalil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\PROJETS\P-PassionLecture\Passion-Lecture\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C8A16D-BBBC-45BC-9C75-D8941EA6B519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B08B1B1-AAD4-4751-8B19-452239B2B96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -316,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -421,11 +421,89 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -590,80 +668,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1042,7 +1046,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6.9444444444444441E-3</c:v>
@@ -1751,18 +1755,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1958,7 +1962,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2015,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 10 minutes</v>
+        <v>0 jours 3 heurs 0 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2026,15 +2030,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2094,8 +2098,12 @@
       <c r="B8" s="38">
         <v>45369</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="36">
+        <v>2</v>
+      </c>
+      <c r="D8" s="44">
+        <v>50</v>
+      </c>
       <c r="E8" t="s">
         <v>24</v>
       </c>
@@ -2116,8 +2124,8 @@
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="40"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="44"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
       <c r="E9" s="19"/>
       <c r="F9" s="48"/>
       <c r="G9" s="20"/>
@@ -8057,40 +8065,40 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
+      <formula1>$M$7:$M$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C532 C7:C8" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D532 D7:D8" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
-      <formula1>$M$7:$M$15</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8243,7 +8251,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C10" s="49" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8251,7 +8259,7 @@
       </c>
       <c r="D10" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8274,7 +8282,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>4.1666666666666671E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8553,15 +8561,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8571,6 +8570,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8594,14 +8602,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8613,4 +8613,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ajout fichier helpers, commencer a faire la connexion a la db depuis le code
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_MateenKhalil.xlsx
+++ b/Doc/Journal-de-Travail_MateenKhalil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pq40rdc\Documents\GitHub\Passion-Lecture\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B399E4C-2377-4472-9689-2C2902C0D7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B071C0-8CF0-449F-94A5-A407BB2549CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>essaie d'afficher la cover des fichiers epub dans la mainPage (problème au build de l'app ne marche toujours pas)</t>
+  </si>
+  <si>
+    <t>mise en place de docker pour l'api</t>
+  </si>
+  <si>
+    <t>import automatique des fichiers epub dans l'api base de donnée</t>
+  </si>
+  <si>
+    <t>j'ai essayé de faire une requête pour récuperer les livre sur la base de donnée</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1064,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34027777777777779</c:v>
+                  <c:v>0.55902777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1985,8 +1994,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2048,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 12 heurs 9 minutes</v>
+        <v>0 jours 17 heurs 24 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2054,15 +2063,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>480</v>
+        <v>720</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>250</v>
+        <v>325</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>730</v>
+        <v>1045</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2360,10 +2369,19 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="39">
+        <v>45411</v>
+      </c>
       <c r="C18" s="35"/>
-      <c r="D18" s="43"/>
-      <c r="F18" s="48"/>
+      <c r="D18" s="44">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>39</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="O18">
         <v>50</v>
@@ -2372,20 +2390,39 @@
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="40"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="48"/>
+      <c r="C19" s="36">
+        <v>2</v>
+      </c>
+      <c r="D19" s="55">
+        <v>50</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="G19" s="20"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="43"/>
-      <c r="F20" s="48"/>
+      <c r="B20" s="39">
+        <v>45418</v>
+      </c>
+      <c r="C20" s="35">
+        <v>2</v>
+      </c>
+      <c r="D20" s="43">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -8193,7 +8230,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C532 C7:C8" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D532 D7:D8" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D18 D20:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
     </dataValidation>
   </dataValidations>
@@ -8257,11 +8294,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>360</v>
+        <v>600</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>130</v>
+        <v>205</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8269,7 +8306,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.34027777777777779</v>
+        <v>0.55902777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8378,7 +8415,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.4236111111111111</v>
+        <v>0.64236111111111105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
connexion db et info livres
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_MateenKhalil.xlsx
+++ b/Doc/Journal-de-Travail_MateenKhalil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pq40rdc\Documents\GitHub\Passion-Lecture\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B071C0-8CF0-449F-94A5-A407BB2549CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBE1043-B048-472B-A5BC-6BDDBD159755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="6990" yWindow="2505" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>j'ai essayé de faire une requête pour récuperer les livre sur la base de donnée</t>
+  </si>
+  <si>
+    <t>j'ai essayé de communiquer entre la db et l'application (j'ai finis les string de connexion et le code pour récuperer les info et afficher les titres des livre dans la mainPage) pour linstant pas finis et les titre ne s'affichent pas</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1067,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55902777777777779</c:v>
+                  <c:v>0.68402777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1995,7 +1998,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2051,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 17 heurs 24 minutes</v>
+        <v>0 jours 20 heurs 24 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2063,7 +2066,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>720</v>
+        <v>900</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2071,7 +2074,7 @@
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>1045</v>
+        <v>1225</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2425,13 +2428,23 @@
       </c>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="48"/>
+      <c r="B21" s="40">
+        <v>45425</v>
+      </c>
+      <c r="C21" s="36">
+        <v>3</v>
+      </c>
+      <c r="D21" s="44">
+        <v>0</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>42</v>
+      </c>
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -8294,7 +8307,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>600</v>
+        <v>780</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8306,7 +8319,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.55902777777777779</v>
+        <v>0.68402777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8415,7 +8428,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.64236111111111105</v>
+        <v>0.76736111111111105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8694,15 +8707,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8712,6 +8716,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8735,14 +8748,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8754,4 +8759,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>